<commit_message>
Actualizacion concentrado de metricas
</commit_message>
<xml_diff>
--- a/Organización/Métricas y monitoreo/PTL_Concentrado_Métricas.xlsx
+++ b/Organización/Métricas y monitoreo/PTL_Concentrado_Métricas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="0" windowWidth="16605" windowHeight="9435" tabRatio="835" activeTab="2"/>
+    <workbookView xWindow="1470" yWindow="0" windowWidth="16605" windowHeight="9435" tabRatio="835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Desviacion de esfuerzo" sheetId="6" r:id="rId1"/>
@@ -973,6 +973,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1035,6 +1036,30 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1097,6 +1122,30 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1115,11 +1164,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="118269440"/>
-        <c:axId val="118270976"/>
+        <c:axId val="39734656"/>
+        <c:axId val="44273664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="118269440"/>
+        <c:axId val="39734656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1129,7 +1178,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118270976"/>
+        <c:crossAx val="44273664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1137,7 +1186,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118270976"/>
+        <c:axId val="44273664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1148,13 +1197,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118269440"/>
+        <c:crossAx val="39734656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1199,7 +1249,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1263,11 +1312,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="40979072"/>
-        <c:axId val="40620416"/>
+        <c:axId val="181573120"/>
+        <c:axId val="181574656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="40979072"/>
+        <c:axId val="181573120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1277,7 +1326,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40620416"/>
+        <c:crossAx val="181574656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1285,7 +1334,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40620416"/>
+        <c:axId val="181574656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1297,7 +1346,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40979072"/>
+        <c:crossAx val="181573120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1355,7 +1404,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1416,11 +1464,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="178677632"/>
-        <c:axId val="178679168"/>
+        <c:axId val="169693952"/>
+        <c:axId val="169695488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="178677632"/>
+        <c:axId val="169693952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1430,7 +1478,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="178679168"/>
+        <c:crossAx val="169695488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1438,7 +1486,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="178679168"/>
+        <c:axId val="169695488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1450,7 +1498,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="178677632"/>
+        <c:crossAx val="169693952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1503,6 +1551,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1607,11 +1656,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="40709504"/>
-        <c:axId val="40723584"/>
+        <c:axId val="44294528"/>
+        <c:axId val="44296064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="40709504"/>
+        <c:axId val="44294528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1621,7 +1670,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40723584"/>
+        <c:crossAx val="44296064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1629,7 +1678,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40723584"/>
+        <c:axId val="44296064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1642,7 +1691,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40709504"/>
+        <c:crossAx val="44294528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1689,6 +1738,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1879,11 +1929,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="130388736"/>
-        <c:axId val="130390272"/>
+        <c:axId val="133295488"/>
+        <c:axId val="115868800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="130388736"/>
+        <c:axId val="133295488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1893,7 +1943,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130390272"/>
+        <c:crossAx val="115868800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1901,7 +1951,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="130390272"/>
+        <c:axId val="115868800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1912,13 +1962,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130388736"/>
+        <c:crossAx val="133295488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1963,6 +2014,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2067,11 +2119,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="118360704"/>
-        <c:axId val="118370688"/>
+        <c:axId val="40056320"/>
+        <c:axId val="40057856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="118360704"/>
+        <c:axId val="40056320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2081,7 +2133,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118370688"/>
+        <c:crossAx val="40057856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2089,7 +2141,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118370688"/>
+        <c:axId val="40057856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2102,7 +2154,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118360704"/>
+        <c:crossAx val="40056320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2237,11 +2289,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="142341248"/>
-        <c:axId val="142342784"/>
+        <c:axId val="145580032"/>
+        <c:axId val="145581568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="142341248"/>
+        <c:axId val="145580032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2251,7 +2303,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142342784"/>
+        <c:crossAx val="145581568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2259,7 +2311,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142342784"/>
+        <c:axId val="145581568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2270,7 +2322,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142341248"/>
+        <c:crossAx val="145580032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2387,11 +2439,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="130453888"/>
-        <c:axId val="130455424"/>
+        <c:axId val="145599488"/>
+        <c:axId val="145601280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="130453888"/>
+        <c:axId val="145599488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2401,7 +2453,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130455424"/>
+        <c:crossAx val="145601280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2409,7 +2461,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="130455424"/>
+        <c:axId val="145601280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2421,7 +2473,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130453888"/>
+        <c:crossAx val="145599488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2474,7 +2526,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2544,11 +2595,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="142541184"/>
-        <c:axId val="142542720"/>
+        <c:axId val="131841024"/>
+        <c:axId val="131855104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="142541184"/>
+        <c:axId val="131841024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2558,7 +2609,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142542720"/>
+        <c:crossAx val="131855104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2566,7 +2617,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142542720"/>
+        <c:axId val="131855104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2578,7 +2629,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142541184"/>
+        <c:crossAx val="131841024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2702,11 +2753,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="142564736"/>
-        <c:axId val="142566528"/>
+        <c:axId val="145295616"/>
+        <c:axId val="145297408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="142564736"/>
+        <c:axId val="145295616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2716,7 +2767,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142566528"/>
+        <c:crossAx val="145297408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2724,7 +2775,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142566528"/>
+        <c:axId val="145297408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2736,7 +2787,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142564736"/>
+        <c:crossAx val="145295616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2789,7 +2840,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2853,11 +2903,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="166718464"/>
-        <c:axId val="128987904"/>
+        <c:axId val="131876736"/>
+        <c:axId val="131878272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="166718464"/>
+        <c:axId val="131876736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2867,7 +2917,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128987904"/>
+        <c:crossAx val="131878272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2875,7 +2925,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128987904"/>
+        <c:axId val="131878272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2887,7 +2937,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166718464"/>
+        <c:crossAx val="131876736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2930,7 +2980,7 @@
         <xdr:cNvPr id="3" name="2 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2966,7 +3016,7 @@
         <xdr:cNvPr id="5" name="4 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3009,7 +3059,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3047,7 +3097,7 @@
         <xdr:cNvPr id="3" name="2 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3090,7 +3140,7 @@
         <xdr:cNvPr id="5" name="4 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3126,7 +3176,7 @@
         <xdr:cNvPr id="7" name="6 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3167,7 +3217,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3203,7 +3253,7 @@
         <xdr:cNvPr id="5" name="4 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3244,7 +3294,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3287,7 +3337,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3634,8 +3684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V89"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:B27"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3688,8 +3738,12 @@
       <c r="B20" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
+      <c r="C20" s="29">
+        <v>0</v>
+      </c>
+      <c r="D20" s="29">
+        <v>0</v>
+      </c>
       <c r="E20" s="38" t="e">
         <f>(C20-D20)/C20</f>
         <v>#DIV/0!</v>
@@ -3699,8 +3753,12 @@
       <c r="B21" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
+      <c r="C21" s="29">
+        <v>0</v>
+      </c>
+      <c r="D21" s="29">
+        <v>0</v>
+      </c>
       <c r="E21" s="38" t="e">
         <f t="shared" ref="E21" si="0">(C21-D21)/C21</f>
         <v>#DIV/0!</v>
@@ -3710,8 +3768,12 @@
       <c r="B22" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
+      <c r="C22" s="28">
+        <v>0</v>
+      </c>
+      <c r="D22" s="28">
+        <v>0</v>
+      </c>
       <c r="E22" s="39" t="e">
         <f>(C22-D22)/C22</f>
         <v>#DIV/0!</v>
@@ -3721,8 +3783,12 @@
       <c r="B23" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
+      <c r="C23" s="28">
+        <v>0</v>
+      </c>
+      <c r="D23" s="28">
+        <v>0</v>
+      </c>
       <c r="E23" s="39" t="e">
         <f t="shared" ref="E23:E27" si="1">(C23-D23)/C23</f>
         <v>#DIV/0!</v>
@@ -3732,8 +3798,12 @@
       <c r="B24" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="31"/>
+      <c r="C24" s="28">
+        <v>0</v>
+      </c>
+      <c r="D24" s="31">
+        <v>0</v>
+      </c>
       <c r="E24" s="39" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -3743,8 +3813,12 @@
       <c r="B25" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="31"/>
+      <c r="C25" s="28">
+        <v>0</v>
+      </c>
+      <c r="D25" s="31">
+        <v>0</v>
+      </c>
       <c r="E25" s="39" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -3754,8 +3828,12 @@
       <c r="B26" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="31"/>
+      <c r="C26" s="28">
+        <v>0</v>
+      </c>
+      <c r="D26" s="31">
+        <v>0</v>
+      </c>
       <c r="E26" s="39" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -3765,8 +3843,12 @@
       <c r="B27" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="28"/>
-      <c r="D27" s="31"/>
+      <c r="C27" s="28">
+        <v>0</v>
+      </c>
+      <c r="D27" s="31">
+        <v>0</v>
+      </c>
       <c r="E27" s="39" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -4271,8 +4353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E31"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4462,7 +4544,7 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="B2:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Concentrado de metricas actualizado
</commit_message>
<xml_diff>
--- a/Organización/Métricas y monitoreo/PTL_Concentrado_Métricas.xlsx
+++ b/Organización/Métricas y monitoreo/PTL_Concentrado_Métricas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="0" windowWidth="16605" windowHeight="9435" tabRatio="835" activeTab="1"/>
+    <workbookView xWindow="1470" yWindow="0" windowWidth="16605" windowHeight="9435" tabRatio="835" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Desviacion de esfuerzo" sheetId="6" r:id="rId1"/>
@@ -13,7 +13,8 @@
     <sheet name="Apego a Productos" sheetId="3" r:id="rId4"/>
     <sheet name="Física" sheetId="10" r:id="rId5"/>
     <sheet name="Funcional" sheetId="11" r:id="rId6"/>
-    <sheet name="Indice de Satisfacción" sheetId="13" r:id="rId7"/>
+    <sheet name="Crecimiento anual de ventas" sheetId="14" r:id="rId7"/>
+    <sheet name="Indice de Satisfacción" sheetId="13" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621" iterateDelta="1E-4"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="41">
   <si>
     <t>&lt;Periodo&gt;</t>
   </si>
@@ -130,6 +131,24 @@
   </si>
   <si>
     <t>Plan de Calidad</t>
+  </si>
+  <si>
+    <t>Monto Total</t>
+  </si>
+  <si>
+    <t>Fecha de revisión</t>
+  </si>
+  <si>
+    <t>Oriana</t>
+  </si>
+  <si>
+    <t>Marisol</t>
+  </si>
+  <si>
+    <t>Apegó</t>
+  </si>
+  <si>
+    <t>Periodo</t>
   </si>
 </sst>
 </file>
@@ -263,7 +282,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -319,6 +338,65 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="7" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="7" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="7" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="7" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="7" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -425,7 +503,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -527,6 +605,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="5" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="3" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="2" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="97">
@@ -973,7 +1096,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1164,11 +1286,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="39734656"/>
-        <c:axId val="44273664"/>
+        <c:axId val="80093952"/>
+        <c:axId val="85029632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39734656"/>
+        <c:axId val="80093952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1178,7 +1300,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44273664"/>
+        <c:crossAx val="85029632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1186,7 +1308,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44273664"/>
+        <c:axId val="85029632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1197,14 +1319,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39734656"/>
+        <c:crossAx val="80093952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1249,6 +1370,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1312,11 +1434,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="181573120"/>
-        <c:axId val="181574656"/>
+        <c:axId val="189344384"/>
+        <c:axId val="189350272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="181573120"/>
+        <c:axId val="189344384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1326,7 +1448,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181574656"/>
+        <c:crossAx val="189350272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1334,7 +1456,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181574656"/>
+        <c:axId val="189350272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1346,7 +1468,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181573120"/>
+        <c:crossAx val="189344384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1393,6 +1515,622 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Acumulado Quincenal</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Planeado</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Crecimiento anual de ventas'!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Periodo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Crecimiento anual de ventas'!$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>12345</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Real</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Crecimiento anual de ventas'!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Periodo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Crecimiento anual de ventas'!$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>11234</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="118696192"/>
+        <c:axId val="118697984"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="118696192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="118697984"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="118697984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="118696192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-MX"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Ventas totales</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Crecimiento anual de ventas'!$G$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Planeado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Crecimiento anual de ventas'!$G$13:$I$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Monto Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Crecimiento anual de ventas'!$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2424000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Crecimiento anual de ventas'!$H$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Real </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Crecimiento anual de ventas'!$G$13:$I$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Monto Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Crecimiento anual de ventas'!$H$15</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>11234</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="107661568"/>
+        <c:axId val="107669760"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="107661568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="107669760"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="107669760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="107661568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-MX"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Ventas quincenales por vendedor</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Crecimiento anual de ventas'!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Oriana</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Crecimiento anual de ventas'!$B$14:$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Planeado</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Real </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Crecimiento anual de ventas'!$B$16:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>6172.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6123</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Crecimiento anual de ventas'!$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Marisol</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Crecimiento anual de ventas'!$B$14:$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Planeado</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Real </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Crecimiento anual de ventas'!$B$17:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>6172.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5234</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="75"/>
+        <c:overlap val="-25"/>
+        <c:axId val="127778176"/>
+        <c:axId val="128033920"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="127778176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="128033920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="128033920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9525">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="127778176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-MX"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
               <a:rPr lang="es-MX"/>
               <a:t>Índice</a:t>
             </a:r>
@@ -1404,6 +2142,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1464,11 +2203,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="169693952"/>
-        <c:axId val="169695488"/>
+        <c:axId val="189376384"/>
+        <c:axId val="189377920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="169693952"/>
+        <c:axId val="189376384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1478,7 +2217,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169695488"/>
+        <c:crossAx val="189377920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1486,7 +2225,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="169695488"/>
+        <c:axId val="189377920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1498,7 +2237,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169693952"/>
+        <c:crossAx val="189376384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1551,7 +2290,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1656,11 +2394,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="44294528"/>
-        <c:axId val="44296064"/>
+        <c:axId val="140887552"/>
+        <c:axId val="140889088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="44294528"/>
+        <c:axId val="140887552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1670,7 +2408,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44296064"/>
+        <c:crossAx val="140889088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1678,7 +2416,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44296064"/>
+        <c:axId val="140889088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1691,7 +2429,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44294528"/>
+        <c:crossAx val="140887552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1929,11 +2667,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="133295488"/>
-        <c:axId val="115868800"/>
+        <c:axId val="153060096"/>
+        <c:axId val="153061632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="133295488"/>
+        <c:axId val="153060096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1943,7 +2681,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115868800"/>
+        <c:crossAx val="153061632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1951,7 +2689,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115868800"/>
+        <c:axId val="153061632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1962,7 +2700,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133295488"/>
+        <c:crossAx val="153060096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2119,11 +2857,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="40056320"/>
-        <c:axId val="40057856"/>
+        <c:axId val="153074304"/>
+        <c:axId val="153080192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="40056320"/>
+        <c:axId val="153074304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2133,7 +2871,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40057856"/>
+        <c:crossAx val="153080192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2141,7 +2879,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40057856"/>
+        <c:axId val="153080192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2154,7 +2892,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40056320"/>
+        <c:crossAx val="153074304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2201,7 +2939,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2289,11 +3026,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="145580032"/>
-        <c:axId val="145581568"/>
+        <c:axId val="140907648"/>
+        <c:axId val="140909184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="145580032"/>
+        <c:axId val="140907648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2303,7 +3040,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145581568"/>
+        <c:crossAx val="140909184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2311,7 +3048,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145581568"/>
+        <c:axId val="140909184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2322,7 +3059,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145580032"/>
+        <c:crossAx val="140907648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2375,7 +3112,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2439,11 +3175,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="145599488"/>
-        <c:axId val="145601280"/>
+        <c:axId val="140943744"/>
+        <c:axId val="140945280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="145599488"/>
+        <c:axId val="140943744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2453,7 +3189,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145601280"/>
+        <c:crossAx val="140945280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2461,7 +3197,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145601280"/>
+        <c:axId val="140945280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2473,7 +3209,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145599488"/>
+        <c:crossAx val="140943744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2526,6 +3262,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2595,11 +3332,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="131841024"/>
-        <c:axId val="131855104"/>
+        <c:axId val="177262976"/>
+        <c:axId val="177264512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="131841024"/>
+        <c:axId val="177262976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2609,7 +3346,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131855104"/>
+        <c:crossAx val="177264512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2617,7 +3354,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="131855104"/>
+        <c:axId val="177264512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2629,7 +3366,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131841024"/>
+        <c:crossAx val="177262976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2753,11 +3490,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="145295616"/>
-        <c:axId val="145297408"/>
+        <c:axId val="164896128"/>
+        <c:axId val="78779520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="145295616"/>
+        <c:axId val="164896128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2767,7 +3504,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145297408"/>
+        <c:crossAx val="78779520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2775,7 +3512,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145297408"/>
+        <c:axId val="78779520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2787,7 +3524,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145295616"/>
+        <c:crossAx val="164896128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2840,6 +3577,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2903,11 +3641,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="131876736"/>
-        <c:axId val="131878272"/>
+        <c:axId val="189254656"/>
+        <c:axId val="189260544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="131876736"/>
+        <c:axId val="189254656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2917,7 +3655,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131878272"/>
+        <c:crossAx val="189260544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2925,7 +3663,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="131878272"/>
+        <c:axId val="189260544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2937,7 +3675,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131876736"/>
+        <c:crossAx val="189254656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2980,7 +3718,7 @@
         <xdr:cNvPr id="3" name="2 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3016,7 +3754,7 @@
         <xdr:cNvPr id="5" name="4 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3059,7 +3797,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3097,7 +3835,7 @@
         <xdr:cNvPr id="3" name="2 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3140,7 +3878,7 @@
         <xdr:cNvPr id="5" name="4 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3176,7 +3914,7 @@
         <xdr:cNvPr id="7" name="6 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3217,7 +3955,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3253,7 +3991,7 @@
         <xdr:cNvPr id="5" name="4 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3294,7 +4032,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3337,7 +4075,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3361,6 +4099,101 @@
 </file>
 
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>733424</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="1 Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="2 Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1000125</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="8 Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4353,8 +5186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5540,6 +6373,132 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A12:I17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:9" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="G13" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
+    </row>
+    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="44"/>
+      <c r="G14" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="49" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="53">
+        <v>12345</v>
+      </c>
+      <c r="C15" s="53">
+        <v>11234</v>
+      </c>
+      <c r="D15" s="54">
+        <f>(C15 * 100)/B15</f>
+        <v>91.000405022276226</v>
+      </c>
+      <c r="F15" s="45"/>
+      <c r="G15" s="46">
+        <v>2424000</v>
+      </c>
+      <c r="H15" s="43">
+        <f>C15</f>
+        <v>11234</v>
+      </c>
+      <c r="I15" s="42">
+        <f>(H15 * 100)/G15</f>
+        <v>0.46344884488448845</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="46">
+        <f>B15/2</f>
+        <v>6172.5</v>
+      </c>
+      <c r="C16" s="46">
+        <v>6123</v>
+      </c>
+      <c r="D16" s="54">
+        <f>(C16 * 100)/B16</f>
+        <v>99.198055893074113</v>
+      </c>
+      <c r="F16" s="45"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="52"/>
+    </row>
+    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="46">
+        <f>B15/2</f>
+        <v>6172.5</v>
+      </c>
+      <c r="C17" s="46">
+        <v>5234</v>
+      </c>
+      <c r="D17" s="55">
+        <f>(C17 * 100)/B17</f>
+        <v>84.795463750506272</v>
+      </c>
+      <c r="F17" s="45"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="52"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G13:I13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>